<commit_message>
Updated USA model - 2025-08-03 20:11
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SubRES_Tmpl/SubRES_ConvElecATB25.xlsx
+++ b/VerveStacks_USA/SubRES_Tmpl/SubRES_ConvElecATB25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0884CECF-CEE7-428E-A57A-C81924C08493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336FB6E1-B7AE-4B63-94E9-87C5A98845E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{13522B6D-C3F1-804F-9704-F9700E076566}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{13522B6D-C3F1-804F-9704-F9700E076566}"/>
   </bookViews>
   <sheets>
     <sheet name="NREL ATB" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="159">
   <si>
     <t xml:space="preserve">   Solar Photovoltaic with Axis Tracking</t>
   </si>
@@ -1510,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB62923-0077-40C7-9F44-D8D0A8B2D421}">
   <dimension ref="A1:BO77"/>
   <sheetViews>
-    <sheetView topLeftCell="W5" workbookViewId="0">
-      <selection activeCell="AT44" sqref="AT44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5252,7 +5252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CCCAC7-8287-4DF6-84EA-A47CBAE414EC}">
   <dimension ref="A1:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -6773,9 +6773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F8FC00-A009-4A63-ADF9-D8F36AB1AA92}">
   <dimension ref="A3:X50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -7738,31 +7736,24 @@
         <v>27</v>
       </c>
       <c r="K41" s="4">
-        <f>J15</f>
         <v>2022</v>
       </c>
       <c r="L41" s="4">
-        <f t="shared" ref="L41:Q41" si="6">K15</f>
         <v>2025</v>
       </c>
       <c r="M41" s="4">
-        <f t="shared" si="6"/>
         <v>2030</v>
       </c>
       <c r="N41" s="4">
-        <f t="shared" si="6"/>
         <v>2035</v>
       </c>
       <c r="O41" s="4">
-        <f t="shared" si="6"/>
         <v>2040</v>
       </c>
       <c r="P41" s="4">
-        <f t="shared" si="6"/>
         <v>2045</v>
       </c>
       <c r="Q41" s="4">
-        <f t="shared" si="6"/>
         <v>2050</v>
       </c>
       <c r="R41" s="9" t="s">
@@ -7793,40 +7784,32 @@
         <v>24</v>
       </c>
       <c r="G42" s="3"/>
-      <c r="I42" s="4" t="str">
-        <f t="shared" ref="I42:I50" si="7">C42</f>
-        <v>Penalty_StBldRate_EPV-1</v>
+      <c r="I42" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q42" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W42,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A42</f>
-        <v>#REF!</v>
+      <c r="K42" s="21">
+        <v>132.28233640000002</v>
+      </c>
+      <c r="L42" s="21">
+        <v>111.05708010000001</v>
+      </c>
+      <c r="M42" s="21">
+        <v>98.562316899999999</v>
+      </c>
+      <c r="N42" s="21">
+        <v>91.365093999999999</v>
+      </c>
+      <c r="O42" s="21">
+        <v>86.582641600000002</v>
+      </c>
+      <c r="P42" s="21">
+        <v>81.496649200000007</v>
+      </c>
+      <c r="Q42" s="21">
+        <v>76.668243399999994</v>
       </c>
       <c r="R42" s="4">
         <v>20</v>
@@ -7855,40 +7838,32 @@
       <c r="F43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I43" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_EPV-2</v>
+      <c r="I43" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q43" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W43,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A43</f>
-        <v>#REF!</v>
+      <c r="K43" s="21">
+        <v>661.41168200000004</v>
+      </c>
+      <c r="L43" s="21">
+        <v>555.28540050000004</v>
+      </c>
+      <c r="M43" s="21">
+        <v>492.81158449999998</v>
+      </c>
+      <c r="N43" s="21">
+        <v>456.82547</v>
+      </c>
+      <c r="O43" s="21">
+        <v>432.913208</v>
+      </c>
+      <c r="P43" s="21">
+        <v>407.48324600000001</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>383.34121699999997</v>
       </c>
       <c r="R43" s="4">
         <v>20</v>
@@ -7917,40 +7892,32 @@
       <c r="F44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I44" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_EPV-3</v>
+      <c r="I44" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q44" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W44,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A44</f>
-        <v>#REF!</v>
+      <c r="K44" s="21">
+        <v>6614.1168200000002</v>
+      </c>
+      <c r="L44" s="21">
+        <v>5552.8540050000001</v>
+      </c>
+      <c r="M44" s="21">
+        <v>4928.1158450000003</v>
+      </c>
+      <c r="N44" s="21">
+        <v>4568.2546999999995</v>
+      </c>
+      <c r="O44" s="21">
+        <v>4329.1320800000003</v>
+      </c>
+      <c r="P44" s="21">
+        <v>4074.8324600000001</v>
+      </c>
+      <c r="Q44" s="21">
+        <v>3833.4121699999996</v>
       </c>
       <c r="R44" s="4">
         <v>20</v>
@@ -7981,40 +7948,32 @@
         <v>24</v>
       </c>
       <c r="G45" s="3"/>
-      <c r="I45" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_EWN-1</v>
+      <c r="I45" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q45" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W45,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A45</f>
-        <v>#REF!</v>
+      <c r="K45" s="21">
+        <v>141.11771240000002</v>
+      </c>
+      <c r="L45" s="21">
+        <v>134.7630249</v>
+      </c>
+      <c r="M45" s="21">
+        <v>127.2074097</v>
+      </c>
+      <c r="N45" s="21">
+        <v>122.0000488</v>
+      </c>
+      <c r="O45" s="21">
+        <v>119.1305054</v>
+      </c>
+      <c r="P45" s="21">
+        <v>115.7732544</v>
+      </c>
+      <c r="Q45" s="21">
+        <v>112.6993164</v>
       </c>
       <c r="R45" s="4">
         <v>20</v>
@@ -8028,7 +7987,7 @@
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="26">
-        <f t="shared" ref="A46:A50" si="8">A43</f>
+        <f t="shared" ref="A46:A50" si="6">A43</f>
         <v>0.5</v>
       </c>
       <c r="B46" s="24" t="s">
@@ -8044,40 +8003,32 @@
       <c r="F46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I46" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_EWN-2</v>
+      <c r="I46" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q46" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W46,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A46</f>
-        <v>#REF!</v>
+      <c r="K46" s="21">
+        <v>705.58856200000002</v>
+      </c>
+      <c r="L46" s="21">
+        <v>673.81512450000002</v>
+      </c>
+      <c r="M46" s="21">
+        <v>636.03704849999997</v>
+      </c>
+      <c r="N46" s="21">
+        <v>610.00024399999995</v>
+      </c>
+      <c r="O46" s="21">
+        <v>595.65252699999996</v>
+      </c>
+      <c r="P46" s="21">
+        <v>578.86627199999998</v>
+      </c>
+      <c r="Q46" s="21">
+        <v>563.49658199999999</v>
       </c>
       <c r="R46" s="4">
         <v>20</v>
@@ -8091,7 +8042,7 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B47" s="24" t="s">
@@ -8107,40 +8058,32 @@
       <c r="F47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I47" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_EWN-3</v>
+      <c r="I47" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="K47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; K$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; L$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; M$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; N$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; O$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; P$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q47" s="21" t="e">
-        <f ca="1">SUMIF(#REF!,$W47,INDIRECT("tabTechCost[" &amp; Q$41 &amp; "]"))*$A47</f>
-        <v>#REF!</v>
+      <c r="K47" s="21">
+        <v>7055.88562</v>
+      </c>
+      <c r="L47" s="21">
+        <v>6738.151245</v>
+      </c>
+      <c r="M47" s="21">
+        <v>6360.3704849999995</v>
+      </c>
+      <c r="N47" s="21">
+        <v>6100.0024399999993</v>
+      </c>
+      <c r="O47" s="21">
+        <v>5956.5252700000001</v>
+      </c>
+      <c r="P47" s="21">
+        <v>5788.6627200000003</v>
+      </c>
+      <c r="Q47" s="21">
+        <v>5634.9658199999994</v>
       </c>
       <c r="R47" s="4">
         <v>20</v>
@@ -8154,7 +8097,7 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
       <c r="B48" s="24" t="s">
@@ -8171,39 +8114,31 @@
         <v>24</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="I48" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_ESG-1</v>
+      <c r="I48" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>75</v>
       </c>
       <c r="K48" s="21">
-        <f>J$19*$A48</f>
         <v>202.67200000000003</v>
       </c>
       <c r="L48" s="21">
-        <f t="shared" ref="L48:Q48" si="9">K$19*$A48</f>
         <v>208.37987912913169</v>
       </c>
       <c r="M48" s="21">
-        <f t="shared" si="9"/>
         <v>171.23441609167594</v>
       </c>
       <c r="N48" s="21">
-        <f t="shared" si="9"/>
         <v>165.71473115070074</v>
       </c>
       <c r="O48" s="21">
-        <f t="shared" si="9"/>
         <v>160.19504620972555</v>
       </c>
       <c r="P48" s="21">
-        <f t="shared" si="9"/>
         <v>154.67536126875038</v>
       </c>
       <c r="Q48" s="21">
-        <f t="shared" si="9"/>
         <v>149.15567632777524</v>
       </c>
       <c r="R48" s="4">
@@ -8215,7 +8150,7 @@
     </row>
     <row r="49" spans="1:19">
       <c r="A49" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="B49" s="24" t="s">
@@ -8231,39 +8166,31 @@
       <c r="F49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_ESG-2</v>
+      <c r="I49" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="J49" s="25" t="s">
         <v>75</v>
       </c>
       <c r="K49" s="21">
-        <f t="shared" ref="K49:Q50" si="10">J$19*$A49</f>
         <v>1013.36</v>
       </c>
       <c r="L49" s="21">
-        <f t="shared" si="10"/>
         <v>1041.8993956456584</v>
       </c>
       <c r="M49" s="21">
-        <f t="shared" si="10"/>
         <v>856.17208045837958</v>
       </c>
       <c r="N49" s="21">
-        <f t="shared" si="10"/>
         <v>828.57365575350366</v>
       </c>
       <c r="O49" s="21">
-        <f t="shared" si="10"/>
         <v>800.97523104862773</v>
       </c>
       <c r="P49" s="21">
-        <f t="shared" si="10"/>
         <v>773.37680634375181</v>
       </c>
       <c r="Q49" s="21">
-        <f t="shared" si="10"/>
         <v>745.77838163887623</v>
       </c>
       <c r="R49" s="4">
@@ -8275,7 +8202,7 @@
     </row>
     <row r="50" spans="1:19">
       <c r="A50" s="26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B50" s="24" t="s">
@@ -8291,39 +8218,31 @@
       <c r="F50" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v>Penalty_StBldRate_ESG-3</v>
+      <c r="I50" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="J50" s="25" t="s">
         <v>75</v>
       </c>
       <c r="K50" s="21">
-        <f t="shared" si="10"/>
         <v>10133.6</v>
       </c>
       <c r="L50" s="21">
-        <f t="shared" si="10"/>
         <v>10418.993956456583</v>
       </c>
       <c r="M50" s="21">
-        <f t="shared" si="10"/>
         <v>8561.7208045837961</v>
       </c>
       <c r="N50" s="21">
-        <f t="shared" si="10"/>
         <v>8285.7365575350359</v>
       </c>
       <c r="O50" s="21">
-        <f t="shared" si="10"/>
         <v>8009.7523104862776</v>
       </c>
       <c r="P50" s="21">
-        <f t="shared" si="10"/>
         <v>7733.7680634375183</v>
       </c>
       <c r="Q50" s="21">
-        <f t="shared" si="10"/>
         <v>7457.7838163887627</v>
       </c>
       <c r="R50" s="4">

</xml_diff>